<commit_message>
Adds alternate game, Whipped(?); changes players.xlsx
</commit_message>
<xml_diff>
--- a/data/players.xlsx
+++ b/data/players.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">Color</t>
   </si>
@@ -34,19 +34,16 @@
     <t xml:space="preserve">Money</t>
   </si>
   <si>
-    <t xml:space="preserve">Min_Money</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min_Peek</t>
+    <t xml:space="preserve">Ally Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min Ally Number</t>
   </si>
   <si>
     <t xml:space="preserve">Trade</t>
   </si>
   <si>
-    <t xml:space="preserve">Min_Trade</t>
+    <t xml:space="preserve">Min Trade</t>
   </si>
   <si>
     <t xml:space="preserve">red</t>
@@ -187,10 +184,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -223,129 +220,114 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>9</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G2" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>7</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="I3" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>17</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>7</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="I4" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>20</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>6</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>23</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>6</v>
@@ -354,15 +336,12 @@
         <v>4</v>
       </c>
       <c r="F6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="G6" s="0" t="n">
-        <v>3</v>
-      </c>
       <c r="H6" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="I6" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>